<commit_message>
Committing Integrated Changes by Ajay
</commit_message>
<xml_diff>
--- a/src/test/resources/com/sirion/xls/Clause Suite.xlsx
+++ b/src/test/resources/com/sirion/xls/Clause Suite.xlsx
@@ -1,21 +1,188 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="1065" windowWidth="14805" windowHeight="7050" tabRatio="888"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
+    <sheet name="ClauseCreation" sheetId="13" r:id="rId2"/>
+    <sheet name="ClauseWorkflow" sheetId="14" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="47">
+  <si>
+    <t>TCID</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Runmode</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Results</t>
+  </si>
+  <si>
+    <t>Error</t>
+  </si>
+  <si>
+    <t>ClauseCreation</t>
+  </si>
+  <si>
+    <t>clauseCategory</t>
+  </si>
+  <si>
+    <t>clauseName</t>
+  </si>
+  <si>
+    <t>clauseSupplier</t>
+  </si>
+  <si>
+    <t>clauseType</t>
+  </si>
+  <si>
+    <t>clauseContractingEntity</t>
+  </si>
+  <si>
+    <t>clauseTermType</t>
+  </si>
+  <si>
+    <t>clauseContent</t>
+  </si>
+  <si>
+    <t>clauseRiskType</t>
+  </si>
+  <si>
+    <t>clauseIndustryType</t>
+  </si>
+  <si>
+    <t>clauseCompanyPosition</t>
+  </si>
+  <si>
+    <t>clauseAgreementType</t>
+  </si>
+  <si>
+    <t>clauseTransactionType</t>
+  </si>
+  <si>
+    <t>clauseContractServices</t>
+  </si>
+  <si>
+    <t>clauseTCVMin</t>
+  </si>
+  <si>
+    <t>clausetCVMax</t>
+  </si>
+  <si>
+    <t>clauseRegions</t>
+  </si>
+  <si>
+    <t>clauseCountries</t>
+  </si>
+  <si>
+    <t>clauseFunctions</t>
+  </si>
+  <si>
+    <t>clauseServices</t>
+  </si>
+  <si>
+    <t>Auto Renewal</t>
+  </si>
+  <si>
+    <t>clauseHeaderLabel</t>
+  </si>
+  <si>
+    <t>ABC News</t>
+  </si>
+  <si>
+    <t>This ${Agreement} is made and entered into this day ${Effective Date} between ${Contractor} and ${Operator}. Contractor and Operator are also referred to as party and collectively as the parties. Subject to and in consideration of the mutual promises, conditions, and agreements contained herein, the receipt and sufficiency of which are hereby acknowledged, the parties agree as follows:</t>
+  </si>
+  <si>
+    <t>Obligation</t>
+  </si>
+  <si>
+    <t>Fall-back</t>
+  </si>
+  <si>
+    <t>Steady State Support</t>
+  </si>
+  <si>
+    <t>APAC</t>
+  </si>
+  <si>
+    <t>Afghanistan;
+Akrotiri;
+Albania;
+Algeria;
+American Samoa;
+Andorra;
+Angola;
+Anguilla;
+Antarctica;
+Antigua and Barbuda;
+Argentina;
+Armenia;
+Aruba;
+Ashmore and Cartier Islands;
+Australia;
+Austria;
+Azerbaijan</t>
+  </si>
+  <si>
+    <t>ClauseWorkflow</t>
+  </si>
+  <si>
+    <t>IT;
+Human Resources</t>
+  </si>
+  <si>
+    <t>Applications Development &amp; Maintenance;
+End-User Computing</t>
+  </si>
+  <si>
+    <t>Confidentiality</t>
+  </si>
+  <si>
+    <t>Legal Risk</t>
+  </si>
+  <si>
+    <t>Automobiles &amp; Components</t>
+  </si>
+  <si>
+    <t>Master Service Agreement</t>
+  </si>
+  <si>
+    <t>Sales</t>
+  </si>
+  <si>
+    <t>SKIP</t>
+  </si>
+  <si>
+    <t>Confidentiality - ABC News</t>
+  </si>
+  <si>
+    <t>testCaseId</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -23,16 +190,43 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -40,18 +234,94 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -98,7 +368,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -133,7 +403,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -341,13 +611,370 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" bestFit="true" customWidth="true" style="2" width="15.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="10.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="2" width="7.58203125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="2" width="5.85546875" collapsed="true"/>
+    <col min="6" max="16384" style="2" width="9.140625" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" s="15"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" s="15"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="3"/>
+      <c r="C8" s="3"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
+      <c r="C9" s="3"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:X3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="8" width="10.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="5" width="25.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="8" width="25.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="5" width="15.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="5" width="14.5703125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="5" width="11.28515625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="5" width="23.140625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="5" width="15.85546875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="5" width="15.85546875" collapsed="true"/>
+    <col min="10" max="11" bestFit="true" customWidth="true" style="5" width="14.28515625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="5" width="15.0" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" style="5" width="18.85546875" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" style="5" width="23.28515625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" style="5" width="28.0" collapsed="true"/>
+    <col min="16" max="17" bestFit="true" customWidth="true" style="5" width="22.140625" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" style="5" width="14.28515625" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" style="5" width="14.42578125" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" style="5" width="14.28515625" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" style="5" width="15.7109375" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" style="5" width="10.0" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" style="8" width="7.58203125" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" style="8" width="7.5703125" collapsed="true"/>
+    <col min="25" max="16384" style="5" width="9.140625" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="M1" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="N1" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="O1" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="P1" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q1" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="R1" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="S1" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="T1" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="U1" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="V1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="W1" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="X1" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="7"/>
+      <c r="R2" s="7"/>
+      <c r="S2" s="7"/>
+      <c r="T2" s="7"/>
+      <c r="U2" s="7"/>
+      <c r="V2" s="7"/>
+      <c r="W2" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="X2" s="7"/>
+    </row>
+    <row r="3" spans="1:24" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="11"/>
+      <c r="B3" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="L3" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="M3" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="N3" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="O3" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="P3" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q3" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="R3" s="6">
+        <v>1234567</v>
+      </c>
+      <c r="S3" s="6">
+        <v>123456789</v>
+      </c>
+      <c r="T3" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="U3" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="V3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="W3" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="X3" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="15.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="8" width="14.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="8" width="10.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="8" width="7.58203125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="8" width="5.85546875" collapsed="true"/>
+    <col min="5" max="16384" style="8" width="15.140625" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="7"/>
+    </row>
+    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
committing end user integrated files after client admin integrated files commit
</commit_message>
<xml_diff>
--- a/src/test/resources/com/sirion/xls/Clause Suite.xlsx
+++ b/src/test/resources/com/sirion/xls/Clause Suite.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="48">
   <si>
     <t>TCID</t>
   </si>
@@ -175,6 +175,9 @@
   </si>
   <si>
     <t>PASS</t>
+  </si>
+  <si>
+    <t>FAIL</t>
   </si>
 </sst>
 </file>

</xml_diff>